<commit_message>
updates for bioassay 3/new data
</commit_message>
<xml_diff>
--- a/data/bioassay_3.2.xlsx
+++ b/data/bioassay_3.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741EFBD6-CF49-4B42-BDE2-4734897658FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4D5B45-5DFB-4615-A53F-C7347191E799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{32FA7EB8-539F-49DF-A9B1-534C12AF5415}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{32FA7EB8-539F-49DF-A9B1-534C12AF5415}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B831804-87AE-45DF-92A2-CEE170B4EC7E}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:H9"/>
     </sheetView>
   </sheetViews>
@@ -470,162 +470,162 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>45085</v>
+        <v>45113</v>
       </c>
       <c r="B2">
-        <v>4.3028581391308895</v>
+        <v>4.8896115217396465</v>
       </c>
       <c r="C2">
-        <v>3.4739391680717961</v>
+        <v>3.9476581455361317</v>
       </c>
       <c r="D2">
-        <v>20.802697017374584</v>
+        <v>23.639428428834751</v>
       </c>
       <c r="E2">
-        <v>5.7412802950692958</v>
+        <v>6.5241821534878355</v>
       </c>
       <c r="F2">
-        <v>3.6841100185924374</v>
+        <v>4.186488657491406</v>
       </c>
       <c r="G2">
-        <v>12.986562513089588</v>
+        <v>14.757457401238165</v>
       </c>
       <c r="H2">
-        <v>25.080244428858656</v>
+        <v>28.500277760066652</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>45085</v>
+        <v>45113</v>
       </c>
       <c r="B3">
-        <v>6.3271899504603084</v>
+        <v>4.9431171487971159</v>
       </c>
       <c r="C3">
-        <v>3.6319143274484054</v>
+        <v>4.1271753721004609</v>
       </c>
       <c r="D3">
-        <v>22.168916084804586</v>
+        <v>25.191950096368846</v>
       </c>
       <c r="E3">
-        <v>4.5837401788785455</v>
+        <v>5.2087956578165286</v>
       </c>
       <c r="F3">
-        <v>3.5247916963880264</v>
+        <v>4.0054451095318475</v>
       </c>
       <c r="G3">
-        <v>20.248965533336285</v>
+        <v>23.010188106063957</v>
       </c>
       <c r="H3">
-        <v>24.661209217767368</v>
+        <v>28.024101383826551</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>45085</v>
+        <v>45113</v>
       </c>
       <c r="B4">
-        <v>4.1325383864017002</v>
+        <v>4.6960663481837503</v>
       </c>
       <c r="C4">
-        <v>3.4153694946382989</v>
+        <v>3.8811016984526123</v>
       </c>
       <c r="D4">
-        <v>22.414029619805753</v>
+        <v>25.470488204324724</v>
       </c>
       <c r="E4">
-        <v>4.1342645491105623</v>
+        <v>4.6980278967165479</v>
       </c>
       <c r="F4">
-        <v>3.7056325258521161</v>
+        <v>4.2109460521046769</v>
       </c>
       <c r="G4">
-        <v>21.594890151435798</v>
+        <v>24.539647899358865</v>
       </c>
       <c r="H4">
-        <v>25.489433569490497</v>
+        <v>28.965265419875561</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>45085</v>
+        <v>45113</v>
       </c>
       <c r="B5">
-        <v>4.4487185297295939</v>
+        <v>5.0553619656018114</v>
       </c>
       <c r="C5">
-        <v>3.7247872634535151</v>
+        <v>4.2327127993789944</v>
       </c>
       <c r="D5">
-        <v>24.665043575649015</v>
+        <v>28.028458608692059</v>
       </c>
       <c r="E5">
-        <v>3.91168698514196</v>
+        <v>4.4450988467522272</v>
       </c>
       <c r="F5">
-        <v>3.4802464369182244</v>
+        <v>3.9548254964979823</v>
       </c>
       <c r="G5">
-        <v>23.708008533907361</v>
+        <v>26.940918788531086</v>
       </c>
       <c r="H5">
-        <v>25.171768955032071</v>
+        <v>28.604282903445533</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>45085</v>
+        <v>45113</v>
       </c>
       <c r="B6">
-        <v>4.1476786317221155</v>
+        <v>4.7132711724114937</v>
       </c>
       <c r="C6">
-        <v>4.0153997264526016</v>
+        <v>4.5629542346052281</v>
       </c>
       <c r="D6">
-        <v>26.749623772182144</v>
+        <v>30.397299741116068</v>
       </c>
       <c r="E6">
-        <v>4.6913094256364527</v>
+        <v>5.3310334382232423</v>
       </c>
       <c r="F6">
-        <v>3.5772596545226167</v>
+        <v>4.0650677892302456</v>
       </c>
       <c r="G6">
-        <v>25.744592388922801</v>
+        <v>29.255218623775907</v>
       </c>
       <c r="H6">
-        <v>20.315963866156764</v>
+        <v>23.086322575178144</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>AVERAGE(B2:B6)</f>
-        <v>4.6717967274889221</v>
+        <v>4.8594856313467645</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:H7" si="0">AVERAGE(C2:C6)</f>
-        <v>3.652281996012924</v>
+        <v>4.1503204500146857</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>23.360062013963219</v>
+        <v>26.545525015867288</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>4.6124562867673635</v>
+        <v>5.2414275985992758</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>3.5944080664546845</v>
+        <v>4.0845546209712316</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>20.856603824138364</v>
+        <v>23.700686163793598</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>24.143724007461074</v>
+        <v>27.436050008478492</v>
       </c>
       <c r="I7" t="s">
         <v>8</v>
@@ -638,27 +638,27 @@
       </c>
       <c r="C8">
         <f>C7-B7</f>
-        <v>-1.019514731475998</v>
+        <v>-0.70916518133207873</v>
       </c>
       <c r="D8">
         <f>D7-B7</f>
-        <v>18.688265286474298</v>
+        <v>21.686039384520523</v>
       </c>
       <c r="E8">
         <f>E7-B7</f>
-        <v>-5.9340440721558529E-2</v>
+        <v>0.38194196725251128</v>
       </c>
       <c r="F8">
         <f>F7-B7</f>
-        <v>-1.0773886610342376</v>
+        <v>-0.77493101037553291</v>
       </c>
       <c r="G8">
         <f>G7-B7</f>
-        <v>16.184807096649443</v>
+        <v>18.841200532446834</v>
       </c>
       <c r="H8">
         <f>H7-B7</f>
-        <v>19.471927279972153</v>
+        <v>22.576564377131728</v>
       </c>
       <c r="I8" t="s">
         <v>9</v>
@@ -671,23 +671,23 @@
       </c>
       <c r="D9">
         <f>D7-C7</f>
-        <v>19.707780017950295</v>
+        <v>22.395204565852602</v>
       </c>
       <c r="E9">
         <f>E7-C7</f>
-        <v>0.9601742907544395</v>
+        <v>1.09110714858459</v>
       </c>
       <c r="F9">
         <f>F7-C7</f>
-        <v>-5.7873929558239556E-2</v>
+        <v>-6.5765829043454183E-2</v>
       </c>
       <c r="G9">
         <f>G7-C7</f>
-        <v>17.20432182812544</v>
+        <v>19.550365713778913</v>
       </c>
       <c r="H9">
         <f>H7-C7</f>
-        <v>20.49144201144815</v>
+        <v>23.285729558463807</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B28A743-1D62-4D7A-9943-3F9D76B7C658}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4.6717967274889221</v>
+        <v>4.8594856313467645</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -739,10 +739,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>3.652281996012924</v>
+        <v>4.1503204500146857</v>
       </c>
       <c r="C3">
-        <v>-1.019514731475998</v>
+        <v>-0.70916518133207873</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -753,13 +753,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>23.360062013963219</v>
+        <v>26.545525015867288</v>
       </c>
       <c r="C4">
-        <v>18.688265286474298</v>
+        <v>21.686039384520523</v>
       </c>
       <c r="D4">
-        <v>19.707780017950295</v>
+        <v>22.395204565852602</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -767,13 +767,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.6124562867673635</v>
+        <v>5.2414275985992758</v>
       </c>
       <c r="C5">
-        <v>-5.9340440721558529E-2</v>
+        <v>0.38194196725251128</v>
       </c>
       <c r="D5">
-        <v>0.9601742907544395</v>
+        <v>1.09110714858459</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -781,13 +781,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.5944080664546845</v>
+        <v>4.0845546209712316</v>
       </c>
       <c r="C6">
-        <v>-1.0773886610342376</v>
+        <v>-0.77493101037553291</v>
       </c>
       <c r="D6">
-        <v>-5.7873929558239556E-2</v>
+        <v>-6.5765829043454183E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,13 +795,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>20.856603824138364</v>
+        <v>23.700686163793598</v>
       </c>
       <c r="C7">
-        <v>16.184807096649443</v>
+        <v>18.841200532446834</v>
       </c>
       <c r="D7">
-        <v>17.20432182812544</v>
+        <v>19.550365713778913</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -809,13 +809,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>24.143724007461074</v>
+        <v>27.436050008478492</v>
       </c>
       <c r="C8">
-        <v>19.471927279972153</v>
+        <v>22.576564377131728</v>
       </c>
       <c r="D8">
-        <v>20.49144201144815</v>
+        <v>23.285729558463807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>